<commit_message>
[DOCS] [MODEL] Change num of stations and their chance
</commit_message>
<xml_diff>
--- a/data/charging_stations_summary.xlsx
+++ b/data/charging_stations_summary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SCHOOL\IMS\data\stations_in_Brno\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SCHOOL\IMS\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67C155F-1B65-498B-A041-0150DCBEB02F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03FEFC05-0042-4654-982B-B33CDE39137F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2805" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="16">
   <si>
     <t>ČEZ</t>
   </si>
@@ -78,12 +78,21 @@
   </si>
   <si>
     <t>Ostatní</t>
+  </si>
+  <si>
+    <t>Teplárny</t>
+  </si>
+  <si>
+    <t>%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -93,7 +102,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -130,8 +139,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -343,11 +358,50 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -357,12 +411,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
@@ -429,6 +477,29 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -709,10 +780,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -723,7 +794,7 @@
     <col min="4" max="4" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -737,212 +808,288 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="57" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="58">
+        <v>125</v>
+      </c>
+      <c r="C2" s="59" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="60">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="61"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="63" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="64">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B4" s="54">
         <v>32</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C4" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D4" s="56">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="2" t="s">
+    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="5"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D5" s="6">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="11"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="13" t="s">
+      <c r="J5" s="67" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D6" s="10">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="15" t="s">
+      <c r="F6" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="46">
+        <v>6</v>
+      </c>
+      <c r="I6" s="65">
+        <f>G6/$G$12</f>
+        <v>1.9672131147540985E-2</v>
+      </c>
+      <c r="J6" s="66">
+        <f>I6*100</f>
+        <v>1.9672131147540985</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="16">
+      <c r="B7" s="12">
         <v>36</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C7" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D7" s="14">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="19"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="4" t="s">
+      <c r="F7" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="48">
+        <v>20</v>
+      </c>
+      <c r="I7" s="65">
+        <f t="shared" ref="I7:I11" si="0">G7/$G$12</f>
+        <v>6.5573770491803282E-2</v>
+      </c>
+      <c r="J7" s="66">
+        <f t="shared" ref="J7:J11" si="1">I7*100</f>
+        <v>6.557377049180328</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="15"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="20">
+      <c r="D8" s="16">
         <v>14</v>
       </c>
-      <c r="F6" s="49" t="s">
+      <c r="F8" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="48">
+        <f>77+120</f>
+        <v>197</v>
+      </c>
+      <c r="I8" s="65">
+        <f t="shared" si="0"/>
+        <v>0.64590163934426226</v>
+      </c>
+      <c r="J8" s="66">
+        <f t="shared" si="1"/>
+        <v>64.590163934426229</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="15"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="16">
+        <v>13</v>
+      </c>
+      <c r="F9" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="48">
+        <v>54</v>
+      </c>
+      <c r="I9" s="65">
+        <f t="shared" si="0"/>
+        <v>0.17704918032786884</v>
+      </c>
+      <c r="J9" s="66">
+        <f t="shared" si="1"/>
+        <v>17.704918032786885</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="17"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="20">
+        <v>1</v>
+      </c>
+      <c r="F10" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="48">
+        <v>11</v>
+      </c>
+      <c r="I10" s="65">
+        <f t="shared" si="0"/>
+        <v>3.6065573770491806E-2</v>
+      </c>
+      <c r="J10" s="66">
+        <f t="shared" si="1"/>
+        <v>3.6065573770491808</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="24">
+        <v>47</v>
+      </c>
+      <c r="C11" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="50">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="19"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="4" t="s">
+      <c r="D11" s="26">
+        <v>2</v>
+      </c>
+      <c r="F11" s="49" t="s">
+        <v>12</v>
+      </c>
+      <c r="G11" s="50">
+        <v>17</v>
+      </c>
+      <c r="I11" s="65">
+        <f t="shared" si="0"/>
+        <v>5.5737704918032788E-2</v>
+      </c>
+      <c r="J11" s="66">
+        <f t="shared" si="1"/>
+        <v>5.5737704918032787</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="27"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="28">
+        <v>29</v>
+      </c>
+      <c r="F12" s="51" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="52">
+        <f>SUM(G6:G11)</f>
+        <v>305</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="27"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D13" s="28">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="29"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="32">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="51" t="s">
+      <c r="B15" s="36">
+        <v>58</v>
+      </c>
+      <c r="C15" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="52">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="21"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="23" t="s">
+      <c r="D15" s="38">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="39"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="40">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="39"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="40">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="41"/>
+      <c r="B18" s="42"/>
+      <c r="C18" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="24">
-        <v>1</v>
-      </c>
-      <c r="F8" s="51" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="52">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="27" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="28">
-        <v>47</v>
-      </c>
-      <c r="C9" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="30">
-        <v>2</v>
-      </c>
-      <c r="F9" s="51" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="52">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="31"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="26" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="32">
-        <v>29</v>
-      </c>
-      <c r="F10" s="51" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="52">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="31"/>
-      <c r="B11" s="25"/>
-      <c r="C11" s="26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="32">
-        <v>11</v>
-      </c>
-      <c r="F11" s="53" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="54">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="33"/>
-      <c r="B12" s="34"/>
-      <c r="C12" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="36">
-        <v>5</v>
-      </c>
-      <c r="F12" s="55" t="s">
-        <v>2</v>
-      </c>
-      <c r="G12" s="56">
-        <f>SUM(G6:G11)</f>
-        <v>173</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="39" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" s="40">
-        <v>58</v>
-      </c>
-      <c r="C13" s="41" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="42">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="43"/>
-      <c r="B14" s="37"/>
-      <c r="C14" s="38" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="44">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="43"/>
-      <c r="B15" s="37"/>
-      <c r="C15" s="38" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="44">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="45"/>
-      <c r="B16" s="46"/>
-      <c r="C16" s="47" t="s">
-        <v>10</v>
-      </c>
-      <c r="D16" s="48">
+      <c r="D18" s="44">
         <v>10</v>
       </c>
     </row>

</xml_diff>